<commit_message>
Feat: Added github workflow
</commit_message>
<xml_diff>
--- a/config/Master_Test_Template.xlsx
+++ b/config/Master_Test_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A4952\PycharmProjects\test_automation_project\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D798E6-CADA-4D32-90CF-808AF41638B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA96CD6-9340-4E33-B0BF-A18A815DD1CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10296" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -210,9 +210,6 @@
     <t>contact_info_schema.json</t>
   </si>
   <si>
-    <t>Contact_info.csv</t>
-  </si>
-  <si>
     <t>singleline.json</t>
   </si>
   <si>
@@ -271,18 +268,28 @@
   </si>
   <si>
     <t>transaction_amt</t>
+  </si>
+  <si>
+    <t>Contact_info_21092024.csv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="34">
+  <fonts count="35">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -534,89 +541,92 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -629,17 +639,17 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -943,10 +953,10 @@
   <dimension ref="A1:W39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T2" sqref="T2"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
@@ -1056,7 +1066,7 @@
         <v>25</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>0</v>
@@ -1074,7 +1084,7 @@
         <v>60</v>
       </c>
       <c r="I2" s="33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>0</v>
@@ -1091,14 +1101,14 @@
       <c r="N2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="38" t="s">
-        <v>79</v>
+      <c r="O2" s="44" t="s">
+        <v>78</v>
       </c>
       <c r="P2" s="36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q2" s="37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="R2" s="19"/>
       <c r="S2" s="1" t="s">
@@ -1113,7 +1123,7 @@
         <v>26</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>0</v>
@@ -1131,7 +1141,7 @@
         <v>60</v>
       </c>
       <c r="I3" s="33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>0</v>
@@ -1149,17 +1159,17 @@
         <v>17</v>
       </c>
       <c r="O3" s="38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P3" s="36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q3" s="37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="R3" s="19"/>
       <c r="S3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:23">
@@ -1170,7 +1180,7 @@
         <v>27</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>0</v>
@@ -1188,7 +1198,7 @@
         <v>60</v>
       </c>
       <c r="I4" s="33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>0</v>
@@ -1206,17 +1216,17 @@
         <v>17</v>
       </c>
       <c r="O4" s="38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P4" s="36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q4" s="37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="R4" s="19"/>
       <c r="S4" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:23">
@@ -1227,7 +1237,7 @@
         <v>28</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>0</v>
@@ -1245,7 +1255,7 @@
         <v>60</v>
       </c>
       <c r="I5" s="33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>0</v>
@@ -1263,17 +1273,17 @@
         <v>17</v>
       </c>
       <c r="O5" s="38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P5" s="36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q5" s="37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="R5" s="19"/>
       <c r="S5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:23">
@@ -1284,7 +1294,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>0</v>
@@ -1302,7 +1312,7 @@
         <v>60</v>
       </c>
       <c r="I6" s="33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>0</v>
@@ -1320,17 +1330,17 @@
         <v>17</v>
       </c>
       <c r="O6" s="38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P6" s="36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q6" s="37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="R6" s="19"/>
       <c r="S6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:23">
@@ -1338,10 +1348,10 @@
         <v>44</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>0</v>
@@ -1359,7 +1369,7 @@
         <v>60</v>
       </c>
       <c r="I7" s="33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>0</v>
@@ -1377,17 +1387,17 @@
         <v>17</v>
       </c>
       <c r="O7" s="38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P7" s="36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q7" s="37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="R7" s="19"/>
       <c r="S7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:23">
@@ -1395,10 +1405,10 @@
         <v>50</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>0</v>
@@ -1416,7 +1426,7 @@
         <v>60</v>
       </c>
       <c r="I8" s="33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>0</v>
@@ -1434,17 +1444,17 @@
         <v>17</v>
       </c>
       <c r="O8" s="38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P8" s="36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q8" s="37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="R8" s="19"/>
       <c r="S8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:23">
@@ -1455,7 +1465,7 @@
         <v>28</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>0</v>
@@ -1473,7 +1483,7 @@
         <v>60</v>
       </c>
       <c r="I9" s="33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>0</v>
@@ -1491,28 +1501,28 @@
         <v>17</v>
       </c>
       <c r="O9" s="38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P9" s="36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q9" s="37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="R9" s="19"/>
       <c r="S9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:23">
       <c r="A10" s="40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>0</v>
@@ -1530,7 +1540,7 @@
         <v>60</v>
       </c>
       <c r="I10" s="33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>0</v>
@@ -1548,20 +1558,20 @@
         <v>17</v>
       </c>
       <c r="O10" s="38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P10" s="36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q10" s="37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="R10" s="19"/>
       <c r="S10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T10" s="41" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="U10" s="41"/>
       <c r="V10" s="2">
@@ -1573,13 +1583,13 @@
     </row>
     <row r="11" spans="1:23">
       <c r="A11" s="40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>0</v>
@@ -1597,7 +1607,7 @@
         <v>60</v>
       </c>
       <c r="I11" s="33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>0</v>
@@ -1615,17 +1625,17 @@
         <v>17</v>
       </c>
       <c r="O11" s="38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P11" s="36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q11" s="37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="R11" s="19"/>
       <c r="S11" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:23">
@@ -1636,7 +1646,7 @@
         <v>29</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>45</v>
@@ -1654,7 +1664,7 @@
         <v>17</v>
       </c>
       <c r="I12" s="34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>45</v>
@@ -1682,7 +1692,7 @@
       </c>
       <c r="R12" s="11"/>
       <c r="S12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:23">
@@ -1693,7 +1703,7 @@
         <v>29</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>51</v>
@@ -1711,7 +1721,7 @@
         <v>17</v>
       </c>
       <c r="I13" s="34" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>52</v>
@@ -1739,7 +1749,7 @@
       </c>
       <c r="R13" s="11"/>
       <c r="S13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:23">
@@ -1786,22 +1796,22 @@
         <v>17</v>
       </c>
       <c r="O14" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="P14" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="P14" s="36" t="s">
-        <v>69</v>
-      </c>
       <c r="Q14" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R14" s="11"/>
       <c r="S14" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:23">
       <c r="A15" s="36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>29</v>
@@ -1843,22 +1853,22 @@
         <v>17</v>
       </c>
       <c r="O15" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="P15" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="P15" s="36" t="s">
-        <v>69</v>
-      </c>
       <c r="Q15" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R15" s="11"/>
       <c r="S15" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:23">
       <c r="A16" s="30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>27</v>
@@ -1900,22 +1910,22 @@
         <v>17</v>
       </c>
       <c r="O16" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="P16" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="P16" s="36" t="s">
-        <v>69</v>
-      </c>
       <c r="Q16" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R16" s="11"/>
       <c r="S16" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" s="36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>26</v>
@@ -1957,22 +1967,22 @@
         <v>17</v>
       </c>
       <c r="O17" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="P17" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="P17" s="36" t="s">
-        <v>69</v>
-      </c>
       <c r="Q17" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R17" s="11"/>
       <c r="S17" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:20">
       <c r="A18" s="30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>28</v>
@@ -2014,22 +2024,22 @@
         <v>17</v>
       </c>
       <c r="O18" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="P18" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="P18" s="36" t="s">
-        <v>69</v>
-      </c>
       <c r="Q18" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R18" s="11"/>
       <c r="S18" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:20">
       <c r="A19" s="36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>23</v>
@@ -2071,17 +2081,17 @@
         <v>17</v>
       </c>
       <c r="O19" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="P19" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="P19" s="36" t="s">
-        <v>69</v>
-      </c>
       <c r="Q19" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R19" s="11"/>
       <c r="S19" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:20">
@@ -2506,7 +2516,7 @@
       <c r="S39" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="30" type="noConversion"/>
+  <phoneticPr fontId="31" type="noConversion"/>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S39" xr:uid="{53648117-6315-BD4B-95C3-AF9A5887C458}">
       <formula1>"Y,N"</formula1>

</xml_diff>